<commit_message>
V2.0 - heatmaply inclusion + split up server and ui
</commit_message>
<xml_diff>
--- a/www/moc_data.xlsx
+++ b/www/moc_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\OneDrive - Hogeschool West-Vlaanderen\Dienstverlening-onderzoek\MAniR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthowest-my.sharepoint.com/personal/cedric_hermans2_howest_be/Documents/Dienstverlening-onderzoek/MAniR/ManiR/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEBF549-75E2-4091-AB7A-8EA86188893A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{2EEBF549-75E2-4091-AB7A-8EA86188893A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ECF71F3-57CE-460F-B5E7-04E49311DCE8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7B0BDB0A-AAEE-4044-97F8-24E4CD4FD74D}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{7B0BDB0A-AAEE-4044-97F8-24E4CD4FD74D}"/>
   </bookViews>
   <sheets>
     <sheet name="ANI" sheetId="1" r:id="rId1"/>
     <sheet name="MALDI" sheetId="3" r:id="rId2"/>
+    <sheet name="metadata" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="21">
   <si>
     <t>Sample1</t>
   </si>
@@ -71,6 +72,33 @@
   </si>
   <si>
     <t>Sample12</t>
+  </si>
+  <si>
+    <t>SampleID</t>
+  </si>
+  <si>
+    <t>metadata1</t>
+  </si>
+  <si>
+    <t>metadata2</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>clinical</t>
+  </si>
+  <si>
+    <t>Location 1</t>
+  </si>
+  <si>
+    <t>Location 2</t>
+  </si>
+  <si>
+    <t>Location 3</t>
   </si>
 </sst>
 </file>
@@ -430,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E3A368-BC0B-4477-A737-E0854A1AC03D}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,4 +1548,166 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A692A7-8D07-4B03-AC4C-86BA13023737}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>